<commit_message>
Converged "Customer" and "Employee" table into a "Users" table
</commit_message>
<xml_diff>
--- a/SQL_Tables.xlsx
+++ b/SQL_Tables.xlsx
@@ -5,17 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iv391002\Desktop\Westham Books Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Westham Books Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7644" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6504" windowHeight="4464" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="2" r:id="rId1"/>
-    <sheet name="Customer" sheetId="1" r:id="rId2"/>
-    <sheet name="Employees" sheetId="3" r:id="rId3"/>
-    <sheet name="Billing" sheetId="4" r:id="rId4"/>
+    <sheet name="User" sheetId="1" r:id="rId2"/>
+    <sheet name="Billing" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="75">
   <si>
     <t xml:space="preserve">Field Name </t>
   </si>
@@ -125,9 +124,6 @@
     <t>employeeID</t>
   </si>
   <si>
-    <t>emailAddress</t>
-  </si>
-  <si>
     <t>securityLevel</t>
   </si>
   <si>
@@ -212,21 +208,6 @@
     <t xml:space="preserve">email of customer that made order </t>
   </si>
   <si>
-    <t xml:space="preserve">first name of employee </t>
-  </si>
-  <si>
-    <t>last name of employee</t>
-  </si>
-  <si>
-    <t>7 digit employee identification code. Using varchar instead of int because the leading numbers of 0 (required field) - PRIMARY KEY</t>
-  </si>
-  <si>
-    <t>email address of employee needed for sending reports etc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">security level of employee (super user/regular user) </t>
-  </si>
-  <si>
     <t xml:space="preserve">first name of customer </t>
   </si>
   <si>
@@ -264,6 +245,12 @@
   </si>
   <si>
     <t>expiry date of card in format MM/YY</t>
+  </si>
+  <si>
+    <t>7 digit employee identification code. Using varchar instead of int because the leading numbers of 0 - ONLY FOR EMPLOYEES</t>
+  </si>
+  <si>
+    <t>security level of employee (super user/regular user) - ONLY FOR EMPLOYEES</t>
   </si>
 </sst>
 </file>
@@ -414,7 +401,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="17">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -496,21 +483,6 @@
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -525,42 +497,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C12" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C12" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:C12"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Field " dataDxfId="19"/>
-    <tableColumn id="2" name="Data Type" dataDxfId="18"/>
-    <tableColumn id="3" name="Description" dataDxfId="17"/>
+    <tableColumn id="1" name="Field " dataDxfId="14"/>
+    <tableColumn id="2" name="Data Type" dataDxfId="13"/>
+    <tableColumn id="3" name="Description" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C13" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C13" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:C13"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Field Name " dataDxfId="14"/>
-    <tableColumn id="2" name="Data Type " dataDxfId="13"/>
-    <tableColumn id="3" name="Description" dataDxfId="12"/>
+    <tableColumn id="1" name="Field Name " dataDxfId="9"/>
+    <tableColumn id="2" name="Data Type " dataDxfId="8"/>
+    <tableColumn id="3" name="Description" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:C7" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:C7"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Field " dataDxfId="9"/>
-    <tableColumn id="2" name="Data Type" dataDxfId="8"/>
-    <tableColumn id="3" name="Description" dataDxfId="7"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:C8" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3">
   <autoFilter ref="A1:C8"/>
   <tableColumns count="3">
@@ -872,7 +832,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -902,7 +862,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -913,7 +873,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -924,7 +884,7 @@
         <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -935,7 +895,7 @@
         <v>28</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -946,7 +906,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -957,62 +917,62 @@
         <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1025,10 +985,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1055,7 +1015,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1066,7 +1026,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -1077,7 +1037,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1088,7 +1048,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1099,7 +1059,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1110,7 +1070,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1143,7 +1103,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -1170,13 +1130,33 @@
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1188,97 +1168,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="3" max="3" width="28.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -1306,24 +1195,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1334,51 +1223,51 @@
         <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>